<commit_message>
att pesquisa e funçoes att
</commit_message>
<xml_diff>
--- a/estoque.xlsx
+++ b/estoque.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -442,10 +442,10 @@
         <v>B</v>
       </c>
       <c r="E2" t="str">
-        <v>20842</v>
+        <v>02285</v>
       </c>
       <c r="F2" t="str">
-        <v>MALBEC</v>
+        <v>INTENSE BAS LIQ MATE CAMUFL POP 320 20ml</v>
       </c>
       <c r="G2" t="str">
         <v>6</v>
@@ -456,137 +456,267 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>5</v>
+      </c>
+      <c r="B3" t="str">
         <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1</v>
       </c>
       <c r="C3" t="str">
         <v>3</v>
       </c>
       <c r="D3" t="str">
-        <v>G</v>
+        <v>H</v>
       </c>
       <c r="E3" t="str">
-        <v>54565</v>
+        <v>02286</v>
       </c>
       <c r="F3" t="str">
-        <v>teste</v>
+        <v>INTENSE BAS LIQ MATE CAMUFL POP 330 20ml</v>
       </c>
       <c r="G3" t="str">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="H3" t="str">
-        <v>9</v>
+        <v>asa</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" t="str">
+        <v>6</v>
+      </c>
+      <c r="C4" t="str">
         <v>2</v>
       </c>
-      <c r="C4" t="str">
-        <v>3</v>
-      </c>
       <c r="D4" t="str">
-        <v>H</v>
+        <v>A</v>
       </c>
       <c r="E4" t="str">
-        <v>65465</v>
+        <v>02289</v>
       </c>
       <c r="F4" t="str">
-        <v>asa</v>
+        <v>COMB INTENSE GLITTER CARNAVAL</v>
       </c>
       <c r="G4" t="str">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="H4" t="str">
-        <v>asa</v>
+        <v>psa</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>8</v>
+      </c>
+      <c r="B5" t="str">
+        <v>15</v>
+      </c>
+      <c r="C5" t="str">
+        <v>5</v>
+      </c>
+      <c r="D5" t="str">
+        <v>N</v>
+      </c>
+      <c r="E5" t="str">
+        <v>02483</v>
+      </c>
+      <c r="F5" t="str">
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
+      </c>
+      <c r="G5" t="str">
+        <v>5</v>
+      </c>
+      <c r="H5" t="str">
+        <v>MAKE</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B6" t="str">
+        <v>16</v>
+      </c>
+      <c r="C6" t="str">
         <v>6</v>
       </c>
-      <c r="C5" t="str">
-        <v>2</v>
-      </c>
-      <c r="D5" t="str">
-        <v>A</v>
-      </c>
-      <c r="E5" t="str">
-        <v>54565</v>
-      </c>
-      <c r="F5" t="str">
-        <v>AS</v>
-      </c>
-      <c r="G5" t="str">
-        <v>85</v>
-      </c>
-      <c r="H5" t="str">
-        <v>psa</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <v>9</v>
-      </c>
-      <c r="C6" t="str">
-        <v>5</v>
-      </c>
       <c r="D6" t="str">
-        <v>b</v>
+        <v>N</v>
       </c>
       <c r="E6" t="str">
-        <v>54565</v>
+        <v>02484</v>
       </c>
       <c r="F6" t="str">
-        <v>asas</v>
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
       </c>
       <c r="G6" t="str">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H6" t="str">
-        <v>perf</v>
+        <v>MAKE</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" t="str">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="str">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" t="str">
-        <v>N</v>
+        <v>f</v>
       </c>
       <c r="E7" t="str">
-        <v>92798</v>
+        <v>02485</v>
       </c>
       <c r="F7" t="str">
-        <v>EUDORA SOUL KISS ME BATOM HIDRATANTE BORDÔ LOOK DO DIA 3,7g</v>
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
       </c>
       <c r="G7" t="str">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H7" t="str">
         <v>MAKE</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>8</v>
+      </c>
+      <c r="B8" t="str">
+        <v>18</v>
+      </c>
+      <c r="C8" t="str">
+        <v>8</v>
+      </c>
+      <c r="D8" t="str">
+        <v>G</v>
+      </c>
+      <c r="E8" t="str">
+        <v>02485</v>
+      </c>
+      <c r="F8" t="str">
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
+      </c>
+      <c r="G8" t="str">
+        <v>8</v>
+      </c>
+      <c r="H8" t="str">
+        <v>MAKE</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <v>19</v>
+      </c>
+      <c r="C9" t="str">
+        <v>9</v>
+      </c>
+      <c r="D9" t="str">
+        <v>h</v>
+      </c>
+      <c r="E9" t="str">
+        <v>02485</v>
+      </c>
+      <c r="F9" t="str">
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
+      </c>
+      <c r="G9" t="str">
+        <v>9</v>
+      </c>
+      <c r="H9" t="str">
+        <v>MAKE</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <v>20</v>
+      </c>
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <v>l</v>
+      </c>
+      <c r="E10" t="str">
+        <v>02485</v>
+      </c>
+      <c r="F10" t="str">
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
+      </c>
+      <c r="G10" t="str">
+        <v>10</v>
+      </c>
+      <c r="H10" t="str">
+        <v>MAKE</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="str">
+        <v>21</v>
+      </c>
+      <c r="C11" t="str">
+        <v>11</v>
+      </c>
+      <c r="D11" t="str">
+        <v>q</v>
+      </c>
+      <c r="E11" t="str">
+        <v>02485</v>
+      </c>
+      <c r="F11" t="str">
+        <v>INTENSE LAP P/OLHO POP PRETO 1,1g</v>
+      </c>
+      <c r="G11" t="str">
+        <v>11</v>
+      </c>
+      <c r="H11" t="str">
+        <v>MAKE</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6</v>
+      </c>
+      <c r="B12" t="str">
+        <v>8</v>
+      </c>
+      <c r="C12" t="str">
+        <v>5</v>
+      </c>
+      <c r="D12" t="str">
+        <v>B</v>
+      </c>
+      <c r="E12" t="str">
+        <v>55559</v>
+      </c>
+      <c r="F12" t="str">
+        <v>HER CODE</v>
+      </c>
+      <c r="G12" t="str">
+        <v>12</v>
+      </c>
+      <c r="H12" t="str">
+        <v>PERFUME</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>